<commit_message>
maj excel bruit gaussien
</commit_message>
<xml_diff>
--- a/Rapport/Repartition bruit gaussien.xlsx
+++ b/Rapport/Repartition bruit gaussien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnau\Documents\OneDrive\MEM_One_Drive\2_Ecole - IMT Atlantique\SIT 213 - Atelier logiciel simulation d'un système de transmission\Simulator_2000\Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{FAACA219-0A85-4E04-B339-A27D05B5C182}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{7A354E3B-9031-46A0-B93F-49FB959BA1D8}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{FAACA219-0A85-4E04-B339-A27D05B5C182}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{DF611631-1DDF-4A09-9870-EF94CCFBFDC6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B016E7EE-1FF0-45F6-8B79-A167A9F58B66}"/>
   </bookViews>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Feuil5!$A$1:$A$300</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Feuil5!$A$1:$A$300</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -226,7 +227,7 @@
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:binning intervalClosed="r">
-              <cx:binCount val="15"/>
+              <cx:binCount val="10"/>
             </cx:binning>
           </cx:layoutPr>
         </cx:series>
@@ -893,7 +894,7 @@
         <cdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{466C8436-BE9A-498B-918A-A8A5F0E39479}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84E79902-712C-41FD-966D-0DD65A74D3B8}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>

</xml_diff>